<commit_message>
1. modify SenGokuJiDaiJinButsu 2. add ToDouFuKen/RyouSeiKoku
</commit_message>
<xml_diff>
--- a/戦国時代人物.xlsx
+++ b/戦国時代人物.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19020" windowHeight="4350"/>
+    <workbookView windowWidth="20490" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="戦国時代人物" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367">
   <si>
     <t>織田　信長</t>
   </si>
@@ -213,6 +213,18 @@
 蒸し返す-むしかえす</t>
   </si>
   <si>
+    <t>村井　貞勝</t>
+  </si>
+  <si>
+    <t>むらい　さだかつ</t>
+  </si>
+  <si>
+    <t>織田家臣。家中随一の吏僚。京都所司代を務め、京の治安維持、禁裏の修築などに従事し、主君・信長の内政を助けた。本能寺の変の際、二条御所で戦死した。</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>蒲生　氏郷</t>
   </si>
   <si>
@@ -271,9 +283,6 @@
   </si>
   <si>
     <t>織田家臣。妻・千代の内助の功が著名。本能寺の変後は豊臣秀吉に属す。関ケ原合戦の際は居城・掛川城を徳川家康に献上し、戦後、土佐高知２４万石を得た。</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>不破　光治</t>
@@ -331,6 +340,18 @@
 先立つ-さきだつ</t>
   </si>
   <si>
+    <t>宇喜多　直家</t>
+  </si>
+  <si>
+    <t>うきた　なおいえ</t>
+  </si>
+  <si>
+    <t>浦上家臣。乙子城主。権謀術数の限りを尽くして敵を葬り去り、家中最大の勢力を築き上げる。最後は主君・宗景を追放して備前国を掌握した稀代の謀将。</t>
+  </si>
+  <si>
+    <t>葬り去る-ほうむりさる</t>
+  </si>
+  <si>
     <t>浅野　長政</t>
   </si>
   <si>
@@ -499,6 +520,15 @@
     <t>足止めする-あしどめする</t>
   </si>
   <si>
+    <t>千　利休</t>
+  </si>
+  <si>
+    <t>せん　りきゅう</t>
+  </si>
+  <si>
+    <t>戦国時代の茶人。武野紹鴎から茶の湯を学ぶ。織田信長や豊臣秀吉に茶匠として仕え「わび茶」を大成させるなど活躍したが、秀吉と対立し、自害されられた。</t>
+  </si>
+  <si>
     <t>徳川　家康</t>
   </si>
   <si>
@@ -599,6 +629,18 @@
   <si>
     <t>隠密-おんみつ
 無事-ぶじ</t>
+  </si>
+  <si>
+    <t>南光坊　天海</t>
+  </si>
+  <si>
+    <t>なんこうぼう　てんかい</t>
+  </si>
+  <si>
+    <t>徳川家臣。比叡山で教学を究めた天台宗の僧。主君・家康の側近となり国政に辣腕を振るい「黒衣の宰相」と呼ばれた。明智光秀と同一人物との異説がある。</t>
+  </si>
+  <si>
+    <t>側近-そっきん</t>
   </si>
   <si>
     <t>徳川　秀忠</t>
@@ -622,19 +664,13 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>駿河の戦国大名。異母兄</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="ＭＳ ゴシック"/>
         <charset val="128"/>
       </rPr>
       <t>・</t>
@@ -656,6 +692,15 @@
 断ち-たち</t>
   </si>
   <si>
+    <t>太原　雪斎</t>
+  </si>
+  <si>
+    <t>たいげん　せっさい</t>
+  </si>
+  <si>
+    <t>今川家臣。執権を務めた。小豆坂の合戦で織田軍を破り、甲相駿三国同盟を成立させるなど、主家の政治、文化、経済、軍事、外交すべてに大きく貢献した。</t>
+  </si>
+  <si>
     <t>武田　信玄</t>
   </si>
   <si>
@@ -666,6 +711,30 @@
   </si>
   <si>
     <t>率いる-ひきいる</t>
+  </si>
+  <si>
+    <t>山県　昌景</t>
+  </si>
+  <si>
+    <t>やまがた　まさかげ</t>
+  </si>
+  <si>
+    <t>武田家臣。武田四名臣の１人。兄・飯富虎昌と同様、軍装を赤で統一。内政・軍事・外交全般で主君・信玄を補佐した。長篠合戦で全身に銃弾を浴び戦死した。</t>
+  </si>
+  <si>
+    <t>浴びる-あびる</t>
+  </si>
+  <si>
+    <t>山本　勘助</t>
+  </si>
+  <si>
+    <t>やまもと　かんすけ</t>
+  </si>
+  <si>
+    <t>武田家臣。文武百般に通じ、主君・信玄の軍師を務めた。第四次川中島の合戦で「啄木鳥の戦法」を上杉謙信に見破られた責を負い、乱軍に突入し戦死した。</t>
+  </si>
+  <si>
+    <t>啄木鳥-きつつき</t>
   </si>
   <si>
     <t>上杉　謙信</t>
@@ -681,6 +750,60 @@
 翻す-ひるがえす</t>
   </si>
   <si>
+    <t>柿崎　景家</t>
+  </si>
+  <si>
+    <t>かきざき　かげいえ</t>
+  </si>
+  <si>
+    <t>上杉家臣。主君・謙信に「越後七郡で彼にかなうものはなし」と評された家中随一の猛将。上杉軍の主力として活躍したが織田信長への内通疑惑により殺された。</t>
+  </si>
+  <si>
+    <t>宇佐美　定満</t>
+  </si>
+  <si>
+    <t>うさみ　さだみつ</t>
+  </si>
+  <si>
+    <t>上杉家臣。越後流軍学の祖という。上条定憲の乱の際は上条方に属すが、定憲の死後、帰参。国政に参画するなど活躍したが、長尾政景と舟遊び中に溺死した。</t>
+  </si>
+  <si>
+    <t>溺死-できし</t>
+  </si>
+  <si>
+    <t>直江　兼続</t>
+  </si>
+  <si>
+    <t>なおえ　かねつぐ</t>
+  </si>
+  <si>
+    <t>上杉家臣。筆頭家老を務めた。豊臣秀吉の評価は高く、陪臣ながら出羽米沢３０万石を領した。関ケ原合戦の際は西軍に属し、徳川家康に「直江状」を放った。</t>
+  </si>
+  <si>
+    <t>斎藤　道三</t>
+  </si>
+  <si>
+    <t>さいとう　どうさん</t>
+  </si>
+  <si>
+    <t>「蝮」の異名をとった美濃の戦国大名。僧から油商人に転身、次いで美濃守護・土岐頼芸に仕官、頼芸を追放して国主となった。のちに子・義龍と戦い、敗死。</t>
+  </si>
+  <si>
+    <t>蝮-まむし</t>
+  </si>
+  <si>
+    <t>足利　義昭</t>
+  </si>
+  <si>
+    <t>あしかが　よしあき</t>
+  </si>
+  <si>
+    <t>室町幕府１５代将軍。織田信長の後援で将軍役に就くがのちに対立、周辺諸国と協力して信長包囲網を敷く。自らも挙兵するが信長軍に敗れ、京を追われた。</t>
+  </si>
+  <si>
+    <t>敷く-しく</t>
+  </si>
+  <si>
     <t>細川　藤孝</t>
   </si>
   <si>
@@ -694,6 +817,15 @@
 命脈-めいみゃく</t>
   </si>
   <si>
+    <t>三好　長慶</t>
+  </si>
+  <si>
+    <t>みよし　ながよし</t>
+  </si>
+  <si>
+    <t>細川家臣。主家の実権を奪って勢力を拡げ、主君・晴元を追放して畿内の掌握に成功した。しかし嫡男・義興や弟たちの死後は心身に支障をきたし、病死した。</t>
+  </si>
+  <si>
     <t>松永　久秀</t>
   </si>
   <si>
@@ -707,13 +839,362 @@
 蜘蛛-くも</t>
   </si>
   <si>
+    <t>浅井　長政</t>
+  </si>
+  <si>
+    <t>あざい　ながまさ</t>
+  </si>
+  <si>
+    <t>近江の戦国大名。小谷城主。久政の子。織田信長の妹・市を娶るが、朝倉家との友誼を重んじ信長と敵対。居城を攻められ、市と娘たちを信長に託し自害した。</t>
+  </si>
+  <si>
+    <t>託する-たくする</t>
+  </si>
+  <si>
+    <t>朝倉　義景</t>
+  </si>
+  <si>
+    <t>あさくら　よしかげ</t>
+  </si>
+  <si>
+    <t>朝倉家５代当主。孝景の嫡男。将軍・足利義昭と結び織田信長包囲網の一角を担うが、次第に勢威を失う。刀根坂合戦で敗北を喫し、一族に背かれて自害した。</t>
+  </si>
+  <si>
+    <t>刀-かたな
+背く-そむく</t>
+  </si>
+  <si>
+    <t>朝倉　宗滴</t>
+  </si>
+  <si>
+    <t>あさくら　そうてき</t>
+  </si>
+  <si>
+    <t>朝倉家臣。朝倉家初代当主・敏景の子。軍奉行を務め、周辺諸国へ出兵し朝倉家の武威を内外に知らしめた。加賀一向一揆討伐の際に発病、帰国後に死去した。</t>
+  </si>
+  <si>
+    <t>六角　定頼</t>
+  </si>
+  <si>
+    <t>ろっかく　さだより</t>
+  </si>
+  <si>
+    <t>近江の戦国大名。近江に逃れた将軍・足利義晴を支援した。楽市楽座の創始や、一国一城令の先駆をなす「城割り」を初めて行った人物として著名。</t>
+  </si>
+  <si>
+    <t>逃れる-のがれる</t>
+  </si>
+  <si>
+    <t>島　左近</t>
+  </si>
+  <si>
+    <t>しま　さこん</t>
+  </si>
+  <si>
+    <t>筒井家臣。のち浪人し、石田三成に高禄で召し抱えられる。「三成に過ぎたるもの」と謳われた名将。関ケ原合戦で縦横無尽の活躍をし、壮絶な戦死を遂げた。</t>
+  </si>
+  <si>
+    <t>抱える-かかえる
+謳う-うたう
+壮絶な-そうぜつな</t>
+  </si>
+  <si>
+    <t>本願寺　顕如</t>
+  </si>
+  <si>
+    <t>ほんがんじ　けんにょ</t>
+  </si>
+  <si>
+    <t>本願寺１１世法主。証如の子。武家勢力に抵抗し、日本各地で一向宗門徒を蜂起させる。信長包囲網では中心的役割を担い、十年の長きに渡り戦いを続けた。</t>
+  </si>
+  <si>
+    <t>担う-になう</t>
+  </si>
+  <si>
+    <t>毛利　元就</t>
+  </si>
+  <si>
+    <t>もうり　もとなり</t>
+  </si>
+  <si>
+    <t>安芸の戦国大名。権謀術数を駆使して勢力を拡大、中国１０か国の主となった稀代の謀将。厳島合戦では数々謀略で陶晴賢を翻弄、５倍の兵力の敵を破った。</t>
+  </si>
+  <si>
+    <t>厳島-いつくしま
+翻弄-ほんろう</t>
+  </si>
+  <si>
+    <t>吉川　元春</t>
+  </si>
+  <si>
+    <t>きっかわ　もとはる</t>
+  </si>
+  <si>
+    <t>毛利元就の次男。安芸の豪族・吉川家を継、山陰地方の攻略にあたる。不敗を誇った家中随一の猛将である一方、陣中で「太平記」４０巻を写本したという。</t>
+  </si>
+  <si>
+    <t>誇る-ほこる</t>
+  </si>
+  <si>
+    <t>小早川　隆景</t>
+  </si>
+  <si>
+    <t>こばやかわ　たかかげ</t>
+  </si>
+  <si>
+    <t>毛利元就の三男。安芸の豪族・小早川家を継ぎ、山陽地方の攻略に当たる。本能寺の変後は毛利家の存続をはかって豊臣秀吉に接近し、五大老の１人となった。</t>
+  </si>
+  <si>
+    <t>尼子　経久</t>
+  </si>
+  <si>
+    <t>あまご　つねひさ</t>
+  </si>
+  <si>
+    <t>出雲の戦国大名。京極家に仕えるが、所領押領の罪で出雲守護代を罷免される。のちに居城・月山富田城を奪回して勢力を広げ、中国１１カ国の太守となった。</t>
+  </si>
+  <si>
+    <t>山中　鹿之介</t>
+  </si>
+  <si>
+    <t>やまなか　しかのすけ</t>
+  </si>
+  <si>
+    <t>尼子家臣。三日月に対し「我に七難八苦を…」と願ったという。尼子勝久を擁して主家再興を企むが、播磨上月城で毛利軍に敗れ、安芸への護送中に殺された。</t>
+  </si>
+  <si>
+    <t>企む-たくらむ</t>
+  </si>
+  <si>
+    <t>鈴木　重秀</t>
+  </si>
+  <si>
+    <t>すずき　しげひで</t>
+  </si>
+  <si>
+    <t>紀伊の豪族。佐大夫重意の子。通称「雑賀孫市」。雑賀の鉄砲衆を率いて石山本願寺に入り、織田信長の軍を苦しめた。石山開城後は豊臣秀吉に仕えたという。</t>
+  </si>
+  <si>
+    <t>長宗我部　元親</t>
+  </si>
+  <si>
+    <t>ちょうそかべ　もとちか</t>
+  </si>
+  <si>
+    <t>土佐の戦国大名。岡豊城主。国親の子。剽悍の一領具足衆を率い、瞬く間に周辺諸国を制圧。１０数年で四国統一を成し遂げ「土佐の出来人」の異名をとった。</t>
+  </si>
+  <si>
+    <t>成し遂げる-なしとげる</t>
+  </si>
+  <si>
+    <t>島津　義久</t>
+  </si>
+  <si>
+    <t>しまづ　よしひさ</t>
+  </si>
+  <si>
+    <t>島津家１６代当主。貴久の嫡男。優秀な弟たちの協力により領土を拡大、九州をほぼ手中に収めるが、豊臣秀吉の九州征伐軍に敗北し、薩摩１国を安堵された。</t>
+  </si>
+  <si>
     <t>島津　義弘</t>
   </si>
   <si>
-    <t>ひまづ　よしひろ</t>
-  </si>
-  <si>
-    <t>島津家１７代当主。貴久の次男。伊東・大友両家を粉砕し、島津家を隆盛に導いた家中随一の猛将。朝鮮派兵の際は明の大軍を破り「」</t>
+    <t>しまづ　よしひろ</t>
+  </si>
+  <si>
+    <t>島津家１７代当主。貴久の次男。伊東・大友両家を粉砕し、島津家を隆盛に導いた家中随一の猛将。朝鮮派兵の際は明の大軍を破り「鬼石曼子」と恐れられた。</t>
+  </si>
+  <si>
+    <t>島津　家久</t>
+  </si>
+  <si>
+    <t>しまづ　いえひさ</t>
+  </si>
+  <si>
+    <t>島津家臣。貴久の四男。永吉島津家の祖となる。沖田畷合戦の際は１０倍の兵力の龍造寺軍を破る。豊臣秀吉の九州征伐に降り、豊臣秀長の会見後に急死。</t>
+  </si>
+  <si>
+    <t>畷-なわて</t>
+  </si>
+  <si>
+    <t>大友　宗麟</t>
+  </si>
+  <si>
+    <t>おおとも　そうりん</t>
+  </si>
+  <si>
+    <t>大友家２１代当主。名は義鎮。義鑑の子。最盛期には九州６カ国を領したが、高城川合戦で島津軍に敗れて家臣を多数失い、以後は没落の一途をなどった。</t>
+  </si>
+  <si>
+    <t>立花　道雪</t>
+  </si>
+  <si>
+    <t>たちばな　どうせつ</t>
+  </si>
+  <si>
+    <t>大友家臣。立花城西城督。落雷で歩行不能となるが、輿を乗って常に大友軍の先陣を切り「鬼道雪」の異名をとった。生涯を軍陣で過ごした、家中随一の猛将。</t>
+  </si>
+  <si>
+    <t>落雷-らくらい
+輿-こし</t>
+  </si>
+  <si>
+    <t>高橋　紹運</t>
+  </si>
+  <si>
+    <t>たかはし　じょううん</t>
+  </si>
+  <si>
+    <t>大友家臣。筑前岩屋城主。吉弘鑑理の次男。立花道雪と双璧をなした猛将。島津軍５万軍勢を居城にてわずか７百の兵で迎撃、敵兵多数を道連れに玉砕した。</t>
+  </si>
+  <si>
+    <t>双璧-そうへき</t>
+  </si>
+  <si>
+    <t>立花　宗茂</t>
+  </si>
+  <si>
+    <t>たちばな　むねしげ</t>
+  </si>
+  <si>
+    <t>大友家臣。高橋紹運の子。立花道雪の娘を娶る。豊臣秀吉に「忠義と剛勇は鎮西一」と評された。関ケ原合戦で西軍に属して改易されるが、のち旧領に復した。</t>
+  </si>
+  <si>
+    <t>龍造寺　隆信</t>
+  </si>
+  <si>
+    <t>りゅうぞうじ　たかのぶ</t>
+  </si>
+  <si>
+    <t>龍造寺家１９代当主。周家の子。村中・水ケ江両家を統一して勢力を拡大し、九州５カ国２島を領した「肥前の熊」。沖田畷合戦で島津軍に大敗し、戦死した。</t>
+  </si>
+  <si>
+    <t>鍋島　直茂</t>
+  </si>
+  <si>
+    <t>なべしま　なおしげ</t>
+  </si>
+  <si>
+    <t>龍造寺家臣。清房の子。主家の発展に貢献した知勇兼備の将。主君・政家を後見して国政を執った。関ケ原合戦で東軍に属し、戦後、肥前の支配権を獲得した。</t>
+  </si>
+  <si>
+    <t>執る-とる
+獲得-かくとく</t>
+  </si>
+  <si>
+    <t>北条　氏綱</t>
+  </si>
+  <si>
+    <t>北条　うじつな</t>
+  </si>
+  <si>
+    <t>後北条家２代当主。「北条」の姓を初めて使用した。扇ケ谷上杉家の戦いや、小弓公方・足利家との第一次国府台合戦に勝つなど、着実に関東に地盤を築いた。</t>
+  </si>
+  <si>
+    <t>扇ヶ谷-おうぎがやつ
+着実-ちゃくじつ
+地盤-じばん</t>
+  </si>
+  <si>
+    <t>北条　氏康</t>
+  </si>
+  <si>
+    <t>ほうじょう　うじやす</t>
+  </si>
+  <si>
+    <t>後北条家３代当主。氏綱の嫡男。武田信玄・上杉謙信ら強豪としのぎを削り関東に一大王国を築いた。知勇兼備の名将で、戦国期随一の民政家としても著名。</t>
+  </si>
+  <si>
+    <t>削る-けずる
+築く-きずく</t>
+  </si>
+  <si>
+    <t>北条　綱成</t>
+  </si>
+  <si>
+    <t>ほうじょう　つなしげ</t>
+  </si>
+  <si>
+    <t>北条家臣。福島正成の子。父の死後、北条氏綱を頼り、氏綱の娘を娶って一門となる。河越合戦などで活躍し、その旗印より「地黄八幡」と呼ばれ畏怖された。</t>
+  </si>
+  <si>
+    <t>地黄八幡-じおうはちまん</t>
+  </si>
+  <si>
+    <t>伊達　政宗</t>
+  </si>
+  <si>
+    <t>だて　まさむね</t>
+  </si>
+  <si>
+    <t>伊達家１７代当主。輝宗の嫡男。瞬く間に周辺諸国を切り従えて２４歳で奥州に覇を唱え「独眼竜」と畏怖された。権謀術数で豊臣・徳川両政権を生き抜いた。</t>
+  </si>
+  <si>
+    <t>瞬く間-またたくま
+畏怖-いふ</t>
+  </si>
+  <si>
+    <t>伊達　成実</t>
+  </si>
+  <si>
+    <t>だて　しげざね</t>
+  </si>
+  <si>
+    <t>伊達家臣。実元の子。「武」の面で主君の政宗を補佐した伊達家中随一の猛将。「英毅大略あり」と評された。晩年には徳川家光に奥州の軍談を語っている。</t>
+  </si>
+  <si>
+    <t>英毅-えいき</t>
+  </si>
+  <si>
+    <t>片倉　小十郎</t>
+  </si>
+  <si>
+    <t>かたくら　こじゅうろう</t>
+  </si>
+  <si>
+    <t>伊達家臣。１９歳で主君・政宗の傅役となり「智」の面で政宗を補佐した智将。豊臣秀吉の小田原征伐に参陣するよう政宗を説得し、伊達家の存続に貢献した。</t>
+  </si>
+  <si>
+    <t>真田　昌幸</t>
+  </si>
+  <si>
+    <t>さなだ　まさゆき</t>
+  </si>
+  <si>
+    <t>幸隆の三男。「表裏比興の者」と豊臣秀吉に評された稀代の謀将。関ケ原へ行軍途中の徳川秀忠３万８千を数千の兵で翻弄し、秀忠軍を信濃に釘付けにした。</t>
+  </si>
+  <si>
+    <t>釘-くぎ</t>
+  </si>
+  <si>
+    <t>真田　幸村</t>
+  </si>
+  <si>
+    <t>さなだ　ゆきむら</t>
+  </si>
+  <si>
+    <t>昌幸の次男。蟄居先の紀伊九度山から大阪城に入り、大坂の陣で寡兵ながらも徳川の大軍を相手に奮戦した。その戦いぶりは「真田日本一の兵」と称賛された。</t>
+  </si>
+  <si>
+    <t>蟄居-ちっきょ</t>
+  </si>
+  <si>
+    <t>最上　義光</t>
+  </si>
+  <si>
+    <t>もがみ　よしあき</t>
+  </si>
+  <si>
+    <t>最上家１１代当主。義守の嫡男。父を隠居させ、弟を殺して当主となる。密約外交や敵重臣の暗殺など、権謀術数の限りを尽くして、最上家最大の版図を築いた。</t>
+  </si>
+  <si>
+    <t>津軽　為信</t>
+  </si>
+  <si>
+    <t>つがる　ためのぶ</t>
+  </si>
+  <si>
+    <t>弘前藩初代藩主。大浦為則の娘を娶る。主家・南部家から独立し、１７年かけて津軽を統一した。豊臣秀吉の小田原征伐に参陣し、正式に津軽の領主となった。</t>
   </si>
 </sst>
 </file>
@@ -736,14 +1217,64 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -764,20 +1295,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -796,37 +1314,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -865,29 +1352,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <name val="ＭＳ ゴシック"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -900,19 +1381,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,49 +1459,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -984,43 +1495,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,13 +1531,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,31 +1549,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,9 +1592,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1136,8 +1637,23 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,15 +1673,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1180,32 +1687,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1214,145 +1695,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1360,10 +1841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1372,7 +1850,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1719,17 +2200,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B2:E55"/>
+  <dimension ref="B2:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="4.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="36.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
@@ -1739,13 +2220,13 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1753,13 +2234,13 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1770,7 +2251,7 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1784,7 +2265,7 @@
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1798,7 +2279,7 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1812,7 +2293,7 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1899,7 +2380,7 @@
       <c r="D13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2026,34 +2507,34 @@
         <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" ht="54" spans="2:5">
       <c r="B23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" ht="54" spans="2:5">
       <c r="B24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2062,41 +2543,41 @@
         <v>90</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" ht="54" spans="2:5">
       <c r="B26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" ht="54" spans="2:5">
       <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" ht="54" spans="2:5">
@@ -2106,10 +2587,10 @@
       <c r="C28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2120,11 +2601,11 @@
       <c r="C29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>78</v>
+      <c r="E29" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="30" ht="54" spans="2:5">
@@ -2134,10 +2615,10 @@
       <c r="C30" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2148,151 +2629,151 @@
       <c r="C31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>115</v>
+      <c r="E31" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" ht="54" spans="2:5">
       <c r="B32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="33" ht="54" spans="2:5">
       <c r="B33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="34" ht="54" spans="2:5">
       <c r="B34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="35" ht="54" spans="2:5">
       <c r="B35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="36" ht="54" spans="2:5">
       <c r="B36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" ht="54" spans="2:5">
       <c r="B37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="38" ht="54" spans="2:5">
       <c r="B38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="39" ht="54" spans="2:5">
       <c r="B39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="40" ht="54" spans="2:5">
       <c r="B40" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="41" ht="54" spans="2:5">
       <c r="B41" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="42" ht="54" spans="2:5">
@@ -2306,63 +2787,63 @@
         <v>157</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" ht="54" spans="2:5">
       <c r="B43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="44" ht="54" spans="2:5">
       <c r="B44" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>166</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" ht="54" spans="2:5">
       <c r="B45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="46" ht="54" spans="2:5">
       <c r="B46" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="47" ht="54" spans="2:5">
@@ -2372,7 +2853,7 @@
       <c r="C47" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2386,106 +2867,725 @@
       <c r="C48" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>179</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>180</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" ht="54" spans="2:5">
       <c r="B49" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>184</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" ht="54" spans="2:5">
       <c r="B50" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="51" ht="54" spans="2:5">
       <c r="B51" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="52" ht="54" spans="2:5">
       <c r="B52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D52" s="2" t="s">
+    </row>
+    <row r="53" ht="54" spans="2:5">
+      <c r="B53" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="53" ht="54" spans="2:5">
-      <c r="B53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="E53" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D53" s="1" t="s">
+    </row>
+    <row r="54" ht="54" spans="2:5">
+      <c r="B54" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="C54" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="54" ht="54" spans="2:5">
-      <c r="B54" s="1" t="s">
+      <c r="D54" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="E54" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D54" s="1" t="s">
+    </row>
+    <row r="55" ht="54" spans="2:5">
+      <c r="B55" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="55" ht="54" spans="2:4">
-      <c r="B55" s="1" t="s">
+      <c r="D55" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="E55" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" ht="54" spans="2:5">
+      <c r="B56" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>207</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" ht="54" spans="2:5">
+      <c r="B57" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" ht="54" spans="2:5">
+      <c r="B58" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" ht="54" spans="2:5">
+      <c r="B59" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" ht="54" spans="2:5">
+      <c r="B60" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" ht="54" spans="2:5">
+      <c r="B61" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" ht="54" spans="2:5">
+      <c r="B62" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" ht="54" spans="2:5">
+      <c r="B63" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" ht="54" spans="2:5">
+      <c r="B64" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="65" ht="54" spans="2:5">
+      <c r="B65" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" ht="54" spans="2:5">
+      <c r="B66" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" ht="54" spans="2:5">
+      <c r="B67" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" ht="54" spans="2:5">
+      <c r="B68" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" ht="54" spans="2:5">
+      <c r="B69" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" ht="54" spans="2:5">
+      <c r="B70" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" ht="54" spans="2:5">
+      <c r="B71" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" ht="54" spans="2:5">
+      <c r="B72" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" ht="54" spans="2:5">
+      <c r="B73" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="74" ht="54" spans="2:5">
+      <c r="B74" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="75" ht="54" spans="2:5">
+      <c r="B75" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="76" ht="54" spans="2:5">
+      <c r="B76" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" ht="54" spans="2:5">
+      <c r="B77" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" ht="54" spans="2:5">
+      <c r="B78" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="79" ht="54" spans="2:5">
+      <c r="B79" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" ht="54" spans="2:5">
+      <c r="B80" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="81" ht="54" spans="2:5">
+      <c r="B81" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" ht="54" spans="2:5">
+      <c r="B82" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" ht="54" spans="2:5">
+      <c r="B83" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" ht="54" spans="2:5">
+      <c r="B84" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" ht="54" spans="2:5">
+      <c r="B85" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="86" ht="54" spans="2:5">
+      <c r="B86" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="87" ht="54" spans="2:5">
+      <c r="B87" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" ht="54" spans="2:5">
+      <c r="B88" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" ht="54" spans="2:5">
+      <c r="B89" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="90" ht="54" spans="2:5">
+      <c r="B90" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="91" ht="54" spans="2:5">
+      <c r="B91" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="92" ht="54" spans="2:5">
+      <c r="B92" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="93" ht="54" spans="2:5">
+      <c r="B93" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="94" ht="54" spans="2:5">
+      <c r="B94" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="95" ht="54" spans="2:5">
+      <c r="B95" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" ht="54" spans="2:5">
+      <c r="B96" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="97" ht="54" spans="2:5">
+      <c r="B97" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="98" ht="54" spans="2:5">
+      <c r="B98" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" ht="54" spans="2:5">
+      <c r="B99" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>